<commit_message>
sixth commit selected travelers
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/ixigoInputdata.xlsx
+++ b/src/test/resources/testData/ixigoInputdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Akila_Laptop\capgemini eclipse\m2\Testing_ixigo\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF3766D1-286D-4C6E-AF11-9C45942404B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD651CA-A8B0-43D4-964B-18E14F2EACF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -67,8 +67,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-14009]dd\ mmmm\ yyyy;@"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="[$-14009]dd\ mmmm\ yyyy;@"/>
+    <numFmt numFmtId="166" formatCode="[$-14009]d\ mmmm\ yyyy;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -109,8 +110,8 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -399,7 +400,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -450,22 +451,22 @@
       <c r="B2">
         <v>8234</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="3">
         <v>45920</v>
       </c>
-      <c r="F2" s="3">
-        <v>45927</v>
-      </c>
-      <c r="G2" s="2">
+      <c r="F2" s="2">
+        <v>45942</v>
+      </c>
+      <c r="G2">
         <v>2</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2">
         <v>1</v>
       </c>
       <c r="I2" t="s">

</xml_diff>

<commit_message>
seventh commit updated search button and validate it navigate to search flights page
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/ixigoInputdata.xlsx
+++ b/src/test/resources/testData/ixigoInputdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Akila_Laptop\capgemini eclipse\m2\Testing_ixigo\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD651CA-A8B0-43D4-964B-18E14F2EACF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C75ED948-DA67-4A25-B14D-E1A1A165F1F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69,7 +69,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-14009]dd\ mmmm\ yyyy;@"/>
-    <numFmt numFmtId="166" formatCode="[$-14009]d\ mmmm\ yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="[$-14009]d\ mmmm\ yyyy;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -111,7 +111,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>

</xml_diff>

<commit_message>
Eighth commit updated searchflights with special fares
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/ixigoInputdata.xlsx
+++ b/src/test/resources/testData/ixigoInputdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Akila_Laptop\capgemini eclipse\m2\Testing_ixigo\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C75ED948-DA67-4A25-B14D-E1A1A165F1F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9826B088-AC36-4DFF-BFC7-B3B686BAF23B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>ValidmobileNumber</t>
   </si>
@@ -61,6 +61,42 @@
   </si>
   <si>
     <t>Economy</t>
+  </si>
+  <si>
+    <t>Studentoffer</t>
+  </si>
+  <si>
+    <t>Chennai</t>
+  </si>
+  <si>
+    <t>Mumbai</t>
+  </si>
+  <si>
+    <t>Student</t>
+  </si>
+  <si>
+    <t>Coimbatore</t>
+  </si>
+  <si>
+    <t>Hyderabad</t>
+  </si>
+  <si>
+    <t>Premium Economy</t>
+  </si>
+  <si>
+    <t>Senior Citizen</t>
+  </si>
+  <si>
+    <t>Punjab</t>
+  </si>
+  <si>
+    <t>Tiruchirapalli</t>
+  </si>
+  <si>
+    <t>Business</t>
+  </si>
+  <si>
+    <t>Armed Forces</t>
   </si>
 </sst>
 </file>
@@ -397,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -412,10 +448,13 @@
     <col min="6" max="6" width="22" customWidth="1"/>
     <col min="7" max="7" width="21.6640625" customWidth="1"/>
     <col min="8" max="8" width="22.21875" customWidth="1"/>
-    <col min="9" max="9" width="13.88671875" customWidth="1"/>
+    <col min="9" max="9" width="16.109375" customWidth="1"/>
+    <col min="10" max="10" width="14.44140625" customWidth="1"/>
+    <col min="11" max="11" width="20" customWidth="1"/>
+    <col min="12" max="12" width="27.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -443,8 +482,11 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>8015332963</v>
       </c>
@@ -471,6 +513,102 @@
       </c>
       <c r="I2" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>8015332963</v>
+      </c>
+      <c r="B3">
+        <v>8234</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="3">
+        <v>45936</v>
+      </c>
+      <c r="F3" s="3">
+        <v>45942</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>8015332963</v>
+      </c>
+      <c r="B4">
+        <v>8234</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="3">
+        <v>45931</v>
+      </c>
+      <c r="F4" s="3">
+        <v>45961</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>8015332963</v>
+      </c>
+      <c r="B5">
+        <v>8234</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="3">
+        <v>46013</v>
+      </c>
+      <c r="F5" s="3">
+        <v>46040</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
nineth commit searching flights using filters
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/ixigoInputdata.xlsx
+++ b/src/test/resources/testData/ixigoInputdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Akila_Laptop\capgemini eclipse\m2\Testing_ixigo\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9826B088-AC36-4DFF-BFC7-B3B686BAF23B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{565CC123-D7CE-4E92-B126-CEE497D891D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>ValidmobileNumber</t>
   </si>
@@ -97,6 +97,24 @@
   </si>
   <si>
     <t>Armed Forces</t>
+  </si>
+  <si>
+    <t>Stopfilter</t>
+  </si>
+  <si>
+    <t>Non-Stop</t>
+  </si>
+  <si>
+    <t>Airlinesfilter</t>
+  </si>
+  <si>
+    <t>Departuretimefilter</t>
+  </si>
+  <si>
+    <t>EARLY_MORNING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6E </t>
   </si>
 </sst>
 </file>
@@ -433,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -452,9 +470,10 @@
     <col min="10" max="10" width="14.44140625" customWidth="1"/>
     <col min="11" max="11" width="20" customWidth="1"/>
     <col min="12" max="12" width="27.88671875" customWidth="1"/>
+    <col min="13" max="13" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -485,8 +504,17 @@
       <c r="J1" t="s">
         <v>12</v>
       </c>
+      <c r="K1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>8015332963</v>
       </c>
@@ -514,8 +542,17 @@
       <c r="I2" t="s">
         <v>11</v>
       </c>
+      <c r="K2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M2" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>8015332963</v>
       </c>
@@ -547,7 +584,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>8015332963</v>
       </c>
@@ -579,7 +616,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>8015332963</v>
       </c>
@@ -613,5 +650,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
tenth commit applied filter updates
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/ixigoInputdata.xlsx
+++ b/src/test/resources/testData/ixigoInputdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Akila_Laptop\capgemini eclipse\m2\Testing_ixigo\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{565CC123-D7CE-4E92-B126-CEE497D891D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26F981F0-2346-4065-BBC9-4CDE6753C9CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -114,7 +114,7 @@
     <t>EARLY_MORNING</t>
   </si>
   <si>
-    <t xml:space="preserve">6E </t>
+    <t>IndiGo</t>
   </si>
 </sst>
 </file>
@@ -454,7 +454,7 @@
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Features commit for booking flight
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/ixigoInputdata.xlsx
+++ b/src/test/resources/testData/ixigoInputdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Akila_Laptop\capgemini eclipse\m2\Testing_ixigo\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26F981F0-2346-4065-BBC9-4CDE6753C9CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E9D9903-0A32-43AF-9EFF-E8575974D543}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -453,8 +453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -516,7 +516,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
-        <v>8015332963</v>
+        <v>9363339066</v>
       </c>
       <c r="B2">
         <v>8234</v>
@@ -554,7 +554,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
-        <v>8015332963</v>
+        <v>9363339066</v>
       </c>
       <c r="B3">
         <v>8234</v>
@@ -586,7 +586,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>8015332963</v>
+        <v>9363339066</v>
       </c>
       <c r="B4">
         <v>8234</v>
@@ -618,7 +618,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>8015332963</v>
+        <v>9363339066</v>
       </c>
       <c r="B5">
         <v>8234</v>

</xml_diff>

<commit_message>
extent report added updated files
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/ixigoInputdata.xlsx
+++ b/src/test/resources/testData/ixigoInputdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Akila_Laptop\capgemini eclipse\m2\Testing_ixigo\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E9D9903-0A32-43AF-9EFF-E8575974D543}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CC8F764-64D5-4EEB-BD14-A74FF644F562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -63,9 +63,6 @@
     <t>Economy</t>
   </si>
   <si>
-    <t>Studentoffer</t>
-  </si>
-  <si>
     <t>Chennai</t>
   </si>
   <si>
@@ -115,6 +112,9 @@
   </si>
   <si>
     <t>IndiGo</t>
+  </si>
+  <si>
+    <t>Specialoffer</t>
   </si>
 </sst>
 </file>
@@ -453,8 +453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -502,16 +502,16 @@
         <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="K1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" t="s">
         <v>26</v>
-      </c>
-      <c r="M1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
@@ -543,13 +543,13 @@
         <v>11</v>
       </c>
       <c r="K2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
@@ -560,10 +560,10 @@
         <v>8234</v>
       </c>
       <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
         <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
       </c>
       <c r="E3" s="3">
         <v>45936</v>
@@ -581,7 +581,7 @@
         <v>11</v>
       </c>
       <c r="J3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
@@ -592,10 +592,10 @@
         <v>8234</v>
       </c>
       <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
         <v>16</v>
-      </c>
-      <c r="D4" t="s">
-        <v>17</v>
       </c>
       <c r="E4" s="3">
         <v>45931</v>
@@ -610,10 +610,10 @@
         <v>0</v>
       </c>
       <c r="I4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" t="s">
         <v>18</v>
-      </c>
-      <c r="J4" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
@@ -624,10 +624,10 @@
         <v>8234</v>
       </c>
       <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
         <v>20</v>
-      </c>
-      <c r="D5" t="s">
-        <v>21</v>
       </c>
       <c r="E5" s="3">
         <v>46013</v>
@@ -642,10 +642,10 @@
         <v>0</v>
       </c>
       <c r="I5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" t="s">
         <v>22</v>
-      </c>
-      <c r="J5" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
successfully completed Ixigo website testing project
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/ixigoInputdata.xlsx
+++ b/src/test/resources/testData/ixigoInputdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Akila_Laptop\capgemini eclipse\m2\Testing_ixigo\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CC8F764-64D5-4EEB-BD14-A74FF644F562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BFD5B9A-024F-4B56-B153-D1EE27A86CB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -453,8 +453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -516,7 +516,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
-        <v>9363339066</v>
+        <v>8015332963</v>
       </c>
       <c r="B2">
         <v>8234</v>
@@ -554,7 +554,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
-        <v>9363339066</v>
+        <v>8015332963</v>
       </c>
       <c r="B3">
         <v>8234</v>
@@ -586,7 +586,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>9363339066</v>
+        <v>8015332963</v>
       </c>
       <c r="B4">
         <v>8234</v>
@@ -618,7 +618,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>9363339066</v>
+        <v>8015332963</v>
       </c>
       <c r="B5">
         <v>8234</v>

</xml_diff>